<commit_message>
Created Bioeconomic Model V6 and updated components V2
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -18,19 +18,19 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="rL2o5KkWjwUb/kl9wvgFBEd3DbTQC88HUF6A+7lh+iw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="Rlhzym1XHg2shyQ/zleIEWKMo2ceCp2u55Rgvr8v4dA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="177">
   <si>
     <t>Equipment</t>
   </si>
   <si>
-    <t>Unit Cost</t>
+    <t>Unit.Cost</t>
   </si>
   <si>
     <t>Lifespan</t>
@@ -126,10 +126,10 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Task Rate</t>
-  </si>
-  <si>
-    <t>Part Time</t>
+    <t>Task.Rate</t>
+  </si>
+  <si>
+    <t>Part.Time</t>
   </si>
   <si>
     <t>Season</t>
@@ -225,19 +225,16 @@
     <t>Vehicle</t>
   </si>
   <si>
-    <t>Price Gallon</t>
-  </si>
-  <si>
-    <t>Usage Trip</t>
-  </si>
-  <si>
-    <t>Additional Trips</t>
+    <t>Price.Gallon</t>
+  </si>
+  <si>
+    <t>Usage.Trip</t>
   </si>
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Unit Type</t>
+    <t>Unit.Type</t>
   </si>
   <si>
     <t>Cost</t>
@@ -255,9 +252,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Lease Type</t>
   </si>
   <si>
@@ -351,25 +345,25 @@
     <t>Y1 Product</t>
   </si>
   <si>
-    <t xml:space="preserve">Product * (1-Y0 Mortality) </t>
+    <t xml:space="preserve">Product * (1-`Y0 Mortality`) </t>
   </si>
   <si>
     <t>Y2 Product</t>
   </si>
   <si>
-    <t>Y1 Product * (1-Y1 Mortality)</t>
+    <t>`Y1 Product` * (1-`Y1 Mortality`)</t>
   </si>
   <si>
     <t>Y3 Product</t>
   </si>
   <si>
-    <t xml:space="preserve">Y2 Product * (1-Y2 Mortality)  </t>
+    <t xml:space="preserve">`Y2 Product` * (1-`Y2 Mortality`)  </t>
   </si>
   <si>
     <t>Y4 Product</t>
   </si>
   <si>
-    <t>Y3 Product * (1-Y3 Mortality)</t>
+    <t>`Y3 Product` * (1-`Y3 Mortality`)</t>
   </si>
   <si>
     <t>Seed Purchase Cost</t>
@@ -426,13 +420,13 @@
     <t>Ear Hanging Droppers</t>
   </si>
   <si>
-    <t>ceiling((Y2 Product/Scallops Per Dropper))</t>
+    <t>ceiling((`Y2 Product`/`Scallops Per Dropper`))</t>
   </si>
   <si>
     <t>Dropper Length</t>
   </si>
   <si>
-    <t>((Scallops Per Dropper*Scallop Spacing)/2 + Dropper Margins)</t>
+    <t>((`Scallops Per Dropper`*`Scallop Spacing`)/2 + `Dropper Margins`)</t>
   </si>
   <si>
     <t>Daily Work Hours</t>
@@ -547,6 +541,9 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>Additional.Trips</t>
   </si>
   <si>
     <t>Fuel.Cost</t>
@@ -2289,19 +2286,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2">
@@ -2309,10 +2306,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -2320,10 +2317,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
@@ -2331,10 +2328,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5">
@@ -2342,10 +2339,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
@@ -2353,7 +2350,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -2364,7 +2361,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -2375,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -2386,7 +2383,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
@@ -2394,10 +2391,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -2408,7 +2405,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -2419,7 +2416,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -2427,10 +2424,10 @@
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
@@ -2441,10 +2438,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15">
@@ -2452,21 +2449,21 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17">
@@ -2474,10 +2471,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="18">
@@ -2485,21 +2482,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3915,8 +3912,7 @@
     <col customWidth="1" min="1" max="1" width="8.71"/>
     <col customWidth="1" min="2" max="2" width="12.29"/>
     <col customWidth="1" min="3" max="3" width="12.57"/>
-    <col customWidth="1" min="4" max="4" width="15.0"/>
-    <col customWidth="1" min="5" max="23" width="8.71"/>
+    <col customWidth="1" min="4" max="22" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -3929,9 +3925,6 @@
       <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -3943,9 +3936,6 @@
       <c r="C2" s="1">
         <v>21.0</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -3956,9 +3946,6 @@
       </c>
       <c r="C3" s="1">
         <v>5.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.0</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -4979,13 +4966,13 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
@@ -4993,7 +4980,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1">
         <v>50.0</v>
@@ -5004,7 +4991,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1">
         <v>0.05</v>
@@ -6027,31 +6014,28 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="26.14"/>
     <col customWidth="1" min="2" max="2" width="13.71"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2">
         <v>1.0</v>
@@ -6059,7 +6043,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2">
         <v>60.0</v>
@@ -6067,7 +6051,7 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1">
         <v>15.0</v>
@@ -6075,7 +6059,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2">
         <v>100000.0</v>
@@ -6083,7 +6067,7 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2">
         <v>2023.0</v>
@@ -6091,7 +6075,7 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1">
         <v>1000.0</v>
@@ -6099,7 +6083,7 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2">
         <v>35000.0</v>
@@ -6107,7 +6091,7 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="2">
         <v>5000.0</v>
@@ -6115,7 +6099,7 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="2">
         <v>1.0</v>
@@ -6123,7 +6107,7 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="2">
         <v>35000.0</v>
@@ -6131,7 +6115,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" s="2">
         <v>15.0</v>
@@ -6139,7 +6123,7 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>38</v>
@@ -6147,26 +6131,26 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -7175,15 +7159,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2">
         <v>4000.0</v>
@@ -7191,7 +7175,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2">
         <v>100.0</v>
@@ -7199,7 +7183,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2">
         <v>250.0</v>
@@ -7207,7 +7191,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2">
         <v>25.0</v>
@@ -7215,7 +7199,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2">
         <v>10.0</v>
@@ -7223,7 +7207,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2">
         <v>10.0</v>
@@ -7231,7 +7215,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2">
         <v>0.125</v>
@@ -7239,7 +7223,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2">
         <v>0.125</v>
@@ -7247,7 +7231,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2">
         <v>0.125</v>
@@ -7255,7 +7239,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="2">
         <v>0.125</v>
@@ -7263,39 +7247,39 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="2">
         <v>0.01</v>
@@ -7303,7 +7287,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="2">
         <v>4.0</v>
@@ -7311,7 +7295,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B18" s="2">
         <v>100.0</v>
@@ -7319,7 +7303,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="2">
         <v>40.0</v>
@@ -7327,7 +7311,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2">
         <v>1200.0</v>
@@ -7335,7 +7319,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="2">
         <v>10.0</v>
@@ -7343,7 +7327,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B22" s="2">
         <v>4.0</v>
@@ -7351,7 +7335,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="2">
         <v>10.0</v>
@@ -7359,7 +7343,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="2">
         <v>10.0</v>
@@ -7367,7 +7351,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B25" s="2">
         <v>25.0</v>
@@ -7375,7 +7359,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" s="2">
         <v>3.0</v>
@@ -7383,7 +7367,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B27" s="2">
         <v>40.0</v>
@@ -7391,7 +7375,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2">
         <v>100.0</v>
@@ -7399,7 +7383,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" s="2">
         <v>1.0</v>
@@ -7407,7 +7391,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2">
         <v>140.0</v>
@@ -7415,7 +7399,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B31" s="2">
         <v>0.5</v>
@@ -7423,7 +7407,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2">
         <v>10.0</v>
@@ -7431,23 +7415,23 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" s="2">
         <v>8.0</v>
@@ -7478,13 +7462,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2">
@@ -7492,13 +7476,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3">
@@ -7506,13 +7490,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4">
@@ -7520,13 +7504,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="5">
@@ -7534,13 +7518,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -7548,13 +7532,13 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -7562,13 +7546,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
@@ -7576,13 +7560,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
@@ -7590,13 +7574,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
@@ -7604,10 +7588,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2">
         <v>1.0</v>
@@ -7618,13 +7602,13 @@
         <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
@@ -7632,13 +7616,13 @@
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13">
@@ -7646,13 +7630,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14">
@@ -7660,13 +7644,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15">
@@ -7674,13 +7658,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -7711,13 +7695,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17">
@@ -7725,13 +7709,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18">
@@ -7739,13 +7723,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19">
@@ -7753,13 +7737,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -7790,13 +7774,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21">
@@ -7804,13 +7788,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22">
@@ -7818,13 +7802,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23">
@@ -7832,13 +7816,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24">
@@ -7846,7 +7830,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -7860,7 +7844,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -7874,7 +7858,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>18</v>
@@ -7911,13 +7895,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28">
@@ -7925,13 +7909,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29">
@@ -7939,13 +7923,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30">
@@ -7953,13 +7937,13 @@
         <v>10</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
@@ -7990,13 +7974,13 @@
         <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32">
@@ -8004,13 +7988,13 @@
         <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33">
@@ -8018,13 +8002,13 @@
         <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34">
@@ -8032,13 +8016,13 @@
         <v>11</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
@@ -8046,13 +8030,13 @@
         <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36">
@@ -8060,10 +8044,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D36" s="2">
         <v>1.0</v>
@@ -8074,10 +8058,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D37" s="2">
         <v>1.0</v>
@@ -8088,10 +8072,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="2">
         <v>1.0</v>
@@ -8102,10 +8086,10 @@
         <v>25</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D39" s="2">
         <v>0.0</v>
@@ -8116,10 +8100,10 @@
         <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2">
         <v>1.0</v>
@@ -8130,10 +8114,10 @@
         <v>27</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D41" s="2">
         <v>0.0</v>
@@ -8144,10 +8128,10 @@
         <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D42" s="2">
         <v>1.0</v>
@@ -8158,10 +8142,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D43" s="7">
         <v>1.0</v>
@@ -8195,13 +8179,13 @@
         <v>20</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45">
@@ -8209,13 +8193,13 @@
         <v>21</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46">
@@ -8223,13 +8207,13 @@
         <v>16</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47">
@@ -8237,13 +8221,13 @@
         <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48">
@@ -8251,13 +8235,13 @@
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -8285,25 +8269,25 @@
         <v>31</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -8329,19 +8313,19 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3">
@@ -8349,13 +8333,13 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4">
@@ -8363,13 +8347,13 @@
         <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5">
@@ -8377,13 +8361,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6">
@@ -8391,13 +8375,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -8427,13 +8411,13 @@
         <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8">
@@ -8441,13 +8425,13 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9">
@@ -8455,13 +8439,13 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
@@ -8469,13 +8453,13 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11">
@@ -8483,13 +8467,13 @@
         <v>57</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -8519,13 +8503,13 @@
         <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13">
@@ -8533,13 +8517,13 @@
         <v>47</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
@@ -8547,13 +8531,13 @@
         <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
@@ -8561,13 +8545,13 @@
         <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16">
@@ -8575,13 +8559,13 @@
         <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -8611,13 +8595,13 @@
         <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18">
@@ -8625,13 +8609,13 @@
         <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19">
@@ -8639,13 +8623,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -8675,13 +8659,13 @@
         <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21">
@@ -8689,13 +8673,13 @@
         <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22">
@@ -8703,13 +8687,13 @@
         <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23">
@@ -8717,13 +8701,13 @@
         <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24">
@@ -8731,13 +8715,13 @@
         <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25">
@@ -8745,13 +8729,13 @@
         <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26">
@@ -8759,13 +8743,13 @@
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27">
@@ -8773,13 +8757,13 @@
         <v>57</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -8809,13 +8793,13 @@
         <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29">
@@ -8823,13 +8807,13 @@
         <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30">
@@ -8837,13 +8821,13 @@
         <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31">
@@ -8851,13 +8835,13 @@
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32">
@@ -8865,13 +8849,13 @@
         <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33">
@@ -8879,13 +8863,13 @@
         <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34">
@@ -8893,13 +8877,13 @@
         <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35">
@@ -8907,13 +8891,13 @@
         <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -8931,7 +8915,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="21.43"/>
+    <col customWidth="1" min="3" max="4" width="21.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8939,13 +8923,16 @@
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2">
@@ -8953,154 +8940,168 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
continued updating of model V6 and integration of work
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -451,13 +451,13 @@
     <t>Y0</t>
   </si>
   <si>
-    <t>Product/`Spat Collector`</t>
-  </si>
-  <si>
-    <t>(Product/`Spat Collector`)/`Collectors Line`</t>
-  </si>
-  <si>
-    <t>((Product/`Spat Collector`)/`Collectors Line`) * `Spat Site Depth`</t>
+    <t>Product/`Wild Spat Collector`</t>
+  </si>
+  <si>
+    <t>(Product/`Wild Spat Collector`)/`Collectors Line`</t>
+  </si>
+  <si>
+    <t>((Product/`Wild Spat Collector`)/`Collectors Line`) * `Spat Site Depth`</t>
   </si>
   <si>
     <t>Product/(`Seed Net Density`*`Lantern Net Tiers`)</t>

</xml_diff>

<commit_message>
Getting there, Labor integrated
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -13,20 +13,19 @@
     <sheet state="visible" name="Fuel_Output" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Maintenance" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="Maintenance_Output" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="Year" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="pov5bRgw1CajhQFlvjgNutDaMUG0G6v//uh11SScOhc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="U5Yad8Sx9nGRkSjHYrXLQZsSTs3dmSAlvHtxBO5SmK8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="203">
   <si>
     <t>VariableName</t>
   </si>
@@ -85,24 +84,24 @@
     <t>Y3</t>
   </si>
   <si>
+    <t>Spat Procurement</t>
+  </si>
+  <si>
+    <t>Wild Spat - Collected</t>
+  </si>
+  <si>
+    <t>Intermediate Culture</t>
+  </si>
+  <si>
+    <t>Intermediate - Lantern Net</t>
+  </si>
+  <si>
     <t>Grow Out Method</t>
   </si>
   <si>
     <t>Ear Hanging</t>
   </si>
   <si>
-    <t>Spat Procurement</t>
-  </si>
-  <si>
-    <t>Wild Spat - Collected</t>
-  </si>
-  <si>
-    <t>Intermediate Culture</t>
-  </si>
-  <si>
-    <t>Intermediate - Lantern Net</t>
-  </si>
-  <si>
     <t>Wild Spat Collector</t>
   </si>
   <si>
@@ -235,6 +234,9 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Item</t>
+  </si>
+  <si>
     <t>Vessel</t>
   </si>
   <si>
@@ -295,6 +297,9 @@
     <t>Scallop Washer</t>
   </si>
   <si>
+    <t>Specialized Equipment</t>
+  </si>
+  <si>
     <t>Scallop Grader</t>
   </si>
   <si>
@@ -616,12 +621,6 @@
     <t>Additional.Trips</t>
   </si>
   <si>
-    <t>Fuel.Cost</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>Unit.Type</t>
   </si>
   <si>
@@ -635,9 +634,6 @@
   </si>
   <si>
     <t>Maintenance.Cost</t>
-  </si>
-  <si>
-    <t>Specialized Equipment</t>
   </si>
 </sst>
 </file>
@@ -737,10 +733,6 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2110,7 +2102,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2136,13 +2127,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>197</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>201</v>
@@ -2153,217 +2144,203 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2677,7 +2654,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="20" width="8.71"/>
+    <col customWidth="1" min="2" max="4" width="8.71"/>
+    <col customWidth="1" min="5" max="5" width="21.14"/>
+    <col customWidth="1" min="6" max="20" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2693,10 +2672,13 @@
       <c r="D1" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3">
         <v>100000.0</v>
@@ -2707,7 +2689,9 @@
       <c r="D2" s="4">
         <v>1.0</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -2726,7 +2710,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1">
         <v>25000.0</v>
@@ -2737,10 +2721,13 @@
       <c r="D3" s="2">
         <v>1.0</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6">
         <v>800.0</v>
@@ -2754,7 +2741,7 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5">
         <v>0.61</v>
@@ -2765,7 +2752,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2">
         <v>0.07</v>
@@ -2776,7 +2763,7 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1">
         <v>0.91</v>
@@ -2787,7 +2774,7 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" s="4">
         <v>1000.0</v>
@@ -2815,7 +2802,7 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2">
         <v>5.0</v>
@@ -2826,7 +2813,7 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2">
         <v>1.5</v>
@@ -2837,7 +2824,7 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3">
         <v>120.0</v>
@@ -2865,7 +2852,7 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1">
         <v>100.0</v>
@@ -2876,7 +2863,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" s="1">
         <v>70.0</v>
@@ -2887,7 +2874,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2">
         <v>20.0</v>
@@ -2898,7 +2885,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" s="7">
         <v>50.0</v>
@@ -2926,7 +2913,7 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" s="1">
         <v>4.0</v>
@@ -2937,7 +2924,7 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1">
         <v>21.67</v>
@@ -2948,7 +2935,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" s="2">
         <v>20.0</v>
@@ -2959,7 +2946,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2">
         <v>0.1</v>
@@ -2970,7 +2957,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2">
         <v>0.001</v>
@@ -2981,7 +2968,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B21" s="2">
         <v>35000.0</v>
@@ -2992,10 +2979,13 @@
       <c r="D21" s="2">
         <v>1.0</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B22" s="2">
         <v>14000.0</v>
@@ -3006,10 +2996,13 @@
       <c r="D22" s="2">
         <v>1.0</v>
       </c>
+      <c r="E22" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2">
         <v>10000.0</v>
@@ -3020,10 +3013,13 @@
       <c r="D23" s="2">
         <v>1.0</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2">
         <v>2000.0</v>
@@ -3034,10 +3030,13 @@
       <c r="D24" s="2">
         <v>0.0</v>
       </c>
+      <c r="E24" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2">
         <v>25000.0</v>
@@ -3048,10 +3047,13 @@
       <c r="D25" s="2">
         <v>1.0</v>
       </c>
+      <c r="E25" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B26" s="2">
         <v>45000.0</v>
@@ -3062,10 +3064,13 @@
       <c r="D26" s="2">
         <v>0.0</v>
       </c>
+      <c r="E26" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" s="2">
         <v>3000.0</v>
@@ -3079,7 +3084,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2">
         <v>2000.0</v>
@@ -3093,7 +3098,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B29" s="2">
         <v>0.01</v>
@@ -4106,10 +4111,10 @@
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>68</v>
@@ -4117,125 +4122,125 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>1.0</v>
@@ -4243,13 +4248,13 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
@@ -4257,58 +4262,58 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -4336,58 +4341,58 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -4415,69 +4420,69 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2">
         <v>1.0</v>
@@ -4485,13 +4490,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2">
         <v>1.0</v>
@@ -4499,13 +4504,13 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="7">
         <v>1.0</v>
@@ -4535,58 +4540,58 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
@@ -4613,83 +4618,83 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2">
         <v>1.0</v>
@@ -4697,13 +4702,13 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D37" s="2">
         <v>1.0</v>
@@ -4711,13 +4716,13 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2">
         <v>1.0</v>
@@ -4725,13 +4730,13 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D39" s="2">
         <v>0.0</v>
@@ -4739,13 +4744,13 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D40" s="2">
         <v>1.0</v>
@@ -4753,13 +4758,13 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D41" s="2">
         <v>0.0</v>
@@ -4767,13 +4772,13 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D42" s="2">
         <v>1.0</v>
@@ -4781,13 +4786,13 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D43" s="7">
         <v>1.0</v>
@@ -4818,72 +4823,72 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4910,27 +4915,27 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1">
         <v>50.0</v>
@@ -4944,10 +4949,10 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1">
         <v>100.0</v>
@@ -4956,15 +4961,15 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1">
         <v>50.0</v>
@@ -4973,15 +4978,15 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1">
         <v>200000.0</v>
@@ -4990,15 +4995,15 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1">
         <v>100.0</v>
@@ -5007,15 +5012,15 @@
         <v>2.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2">
         <v>150.0</v>
@@ -5024,15 +5029,15 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C8" s="1">
         <v>150.0</v>
@@ -5041,15 +5046,15 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C9" s="2">
         <v>150.0</v>
@@ -5058,15 +5063,15 @@
         <v>2.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C10" s="1">
         <v>150.0</v>
@@ -5080,10 +5085,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C11" s="2">
         <v>275.0</v>
@@ -5092,15 +5097,15 @@
         <v>1.0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C12" s="2">
         <v>275.0</v>
@@ -5109,15 +5114,15 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C13" s="2">
         <v>275.0</v>
@@ -5131,10 +5136,10 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C14" s="2">
         <v>8000.0</v>
@@ -5148,10 +5153,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C15" s="2">
         <v>12000.0</v>
@@ -5165,10 +5170,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2">
         <v>10000.0</v>
@@ -5182,10 +5187,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C17" s="2">
         <v>240.0</v>
@@ -5194,15 +5199,15 @@
         <v>0.0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C18" s="1">
         <v>200.0</v>
@@ -5211,15 +5216,15 @@
         <v>0.0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C19" s="2">
         <v>1250.0</v>
@@ -5228,15 +5233,15 @@
         <v>1.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C20" s="2">
         <v>10.0</v>
@@ -5245,15 +5250,15 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C21" s="2">
         <v>0.0</v>
@@ -5267,10 +5272,10 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="C22" s="2">
         <v>0.0</v>
@@ -5279,15 +5284,15 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C23" s="2">
         <v>0.0</v>
@@ -5296,7 +5301,7 @@
         <v>0.0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
@@ -6305,22 +6310,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -6343,102 +6348,102 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -6461,99 +6466,99 @@
     </row>
     <row r="7">
       <c r="A7" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F11" s="7">
         <v>0.0</v>
@@ -6579,99 +6584,99 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F16" s="7">
         <v>0.0</v>
@@ -6697,62 +6702,62 @@
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -6775,159 +6780,159 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F27" s="7">
         <v>0.0</v>
@@ -6953,99 +6958,99 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F32" s="2">
         <v>0.0</v>
@@ -7053,19 +7058,19 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F33" s="2">
         <v>0.0</v>
@@ -7073,19 +7078,19 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F34" s="2">
         <v>0.0</v>
@@ -7093,19 +7098,19 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F35" s="2">
         <v>0.0</v>
@@ -7134,18 +7139,18 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1">
         <v>6.0</v>
@@ -7156,7 +7161,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1">
         <v>4.0</v>
@@ -8183,188 +8188,213 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -8386,7 +8416,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>197</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>198</v>
@@ -8397,18 +8427,18 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50.0</v>
+        <v>165</v>
+      </c>
+      <c r="C2" s="2">
+        <v>150.0</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>200</v>
@@ -8417,7 +8447,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Maintenance is now updated, I will incorporate,  lease setup, growth, and seasonal mortality next
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="205">
   <si>
     <t>VariableName</t>
   </si>
@@ -630,10 +630,16 @@
     <t>Miles</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Maintenance.Cost</t>
+  </si>
+  <si>
+    <t>as.numeric(sum(Labor.Subset[which(Labor.Subset$Year == Maintenance.Subset$Year[i]),6])) * Maintenance.Subset$Cost[i]</t>
+  </si>
+  <si>
+    <t>as.numeric(sum(Labor.Subset[which(Labor.Subset$Year == Maintenance.Subset$Year[i]),6]) * Fuel.Data[which(Fuel.Data$Vehicle == 'Truck'),3]) * Maintenance.Subset$Cost[i]</t>
+  </si>
+  <si>
+    <t>as.numeric(sum(Equipment.Subset[which(Equipment.Subset$Item == 'Specialized Equipment' &amp; Equipment.Subset$Year == Maintenance.Subset$Year[i]),7])) * Maintenance.Subset$Cost[i]</t>
   </si>
 </sst>
 </file>
@@ -2138,9 +2144,6 @@
       <c r="D1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -2152,6 +2155,9 @@
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -2163,6 +2169,9 @@
       <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -2174,6 +2183,9 @@
       <c r="C4" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -2185,6 +2197,9 @@
       <c r="C5" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -2194,7 +2209,10 @@
         <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>85</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="7">
@@ -2205,7 +2223,10 @@
         <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8">
@@ -2218,6 +2239,9 @@
       <c r="C8" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -2229,6 +2253,9 @@
       <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -2240,6 +2267,9 @@
       <c r="C10" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
@@ -2251,6 +2281,9 @@
       <c r="C11" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
@@ -2262,6 +2295,9 @@
       <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
@@ -2273,6 +2309,9 @@
       <c r="C13" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -2284,6 +2323,9 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -2295,6 +2337,9 @@
       <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -2306,6 +2351,9 @@
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
@@ -2317,6 +2365,9 @@
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
@@ -2328,6 +2379,9 @@
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
@@ -2338,6 +2392,9 @@
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -7166,8 +7223,8 @@
       <c r="B3" s="1">
         <v>4.0</v>
       </c>
-      <c r="C3" s="1">
-        <v>5.0</v>
+      <c r="C3" s="2">
+        <v>15.0</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -8411,7 +8468,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="22" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="21.29"/>
+    <col customWidth="1" min="2" max="22" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -8450,6 +8508,12 @@
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2">
+        <v>200.0</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Completed general inputs!  Now we can focus on deliverables.  You'll need to run the Growth_Input first to get the code to work
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -13,19 +13,20 @@
     <sheet state="visible" name="Fuel_Output" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Maintenance" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="Maintenance_Output" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Market" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="U5Yad8Sx9nGRkSjHYrXLQZsSTs3dmSAlvHtxBO5SmK8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="C7Yo+qX2U0KpJo9rIFe9Oc3yJYljr72061amaFkvnls="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="221">
   <si>
     <t>VariableName</t>
   </si>
@@ -252,7 +253,7 @@
     <t>Gangion Line</t>
   </si>
   <si>
-    <t>Mooring Line</t>
+    <t>Mooring Line + Chain</t>
   </si>
   <si>
     <t>Mooring Anchor</t>
@@ -417,6 +418,27 @@
     <t>`Ear Hanging Droppers`* `Dropper Length`</t>
   </si>
   <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>as.numeric((sum(Equipment.Subset[which(Equipment.Subset$Equipment == 'Lantern Net'),7]) * `Lantern Net Spacing`) + (sum(Equipment.Subset[which(Equipment.Subset$Equipment == 'Dropper Line'),7])/`Dropper Length` * `Dropper Line Spacing`))</t>
+  </si>
+  <si>
+    <t>`Longline Quantity` * 2</t>
+  </si>
+  <si>
+    <t>`Longline Quantity`*`Longline Depth`*2*`Mooring Length`</t>
+  </si>
+  <si>
+    <t>`Longline Quantity`*2</t>
+  </si>
+  <si>
+    <t>as.numeric((((sum(Equipment.Subset[which(Equipment.Subset$Equipment == 'Lantern Net'),7]) * `Lantern Net Spacing`) + (sum(Equipment.Subset[which(Equipment.Subset$Equipment == 'Dropper Line'),7])/`Dropper Length` * `Dropper Line Spacing`))/`Surface Float Spacing`)*`Longline Quantity`)</t>
+  </si>
+  <si>
     <t>Task</t>
   </si>
   <si>
@@ -594,12 +616,6 @@
     <t>ceiling(`Ear Hanging Droppers`/Labor.Subset$Task.Rate[i])</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
     <t>`Daily Work Hours` * Market.Product/Labor.Subset$Task.Rate[i]</t>
   </si>
   <si>
@@ -640,13 +656,46 @@
   </si>
   <si>
     <t>as.numeric(sum(Equipment.Subset[which(Equipment.Subset$Item == 'Specialized Equipment' &amp; Equipment.Subset$Year == Maintenance.Subset$Year[i]),7])) * Maintenance.Subset$Cost[i]</t>
+  </si>
+  <si>
+    <t>Market.Product</t>
+  </si>
+  <si>
+    <t>`Y2 Product`</t>
+  </si>
+  <si>
+    <t>`Y2 Product`-(`Y2 Product`*(`Y2 Mortality`/4))</t>
+  </si>
+  <si>
+    <t>`Y2 Product`-(`Y2 Product`*(`Y2 Mortality`/3))</t>
+  </si>
+  <si>
+    <t>`Y2 Product`-(`Y2 Product`*(`Y2 Mortality`/2))</t>
+  </si>
+  <si>
+    <t>`Y3 Product`</t>
+  </si>
+  <si>
+    <t>`Y3 Product`-(`Y3 Product`*(`Y3 Mortality`/4))</t>
+  </si>
+  <si>
+    <t>`Y3 Product`-(`Y3 Product`*(`Y3 Mortality`/3))</t>
+  </si>
+  <si>
+    <t>`Y3 Product`-(`Y3 Product`*(`Y3 Mortality`/2))</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>`Y3 Product`-(`Y3 Product`*(`Y3 Mortality`))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -663,13 +712,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -696,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -716,6 +776,15 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -739,6 +808,10 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2142,7 +2215,7 @@
         <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2">
@@ -2156,7 +2229,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3">
@@ -2170,7 +2243,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4">
@@ -2184,7 +2257,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
@@ -2198,7 +2271,7 @@
         <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6">
@@ -2212,7 +2285,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7">
@@ -2226,7 +2299,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8">
@@ -2240,7 +2313,7 @@
         <v>85</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9">
@@ -2254,7 +2327,7 @@
         <v>85</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10">
@@ -2268,49 +2341,49 @@
         <v>85</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14">
@@ -2324,7 +2397,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15">
@@ -2338,7 +2411,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16">
@@ -2352,49 +2425,174 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2819,7 +3017,7 @@
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="1">
@@ -4542,7 +4740,7 @@
         <v>85</v>
       </c>
       <c r="D24" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
@@ -4556,7 +4754,7 @@
         <v>85</v>
       </c>
       <c r="D25" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
@@ -4570,7 +4768,7 @@
         <v>85</v>
       </c>
       <c r="D26" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -4754,7 +4952,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
@@ -4768,7 +4966,7 @@
         <v>24</v>
       </c>
       <c r="D37" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="38">
@@ -4782,7 +4980,7 @@
         <v>24</v>
       </c>
       <c r="D38" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
@@ -4810,7 +5008,7 @@
         <v>24</v>
       </c>
       <c r="D40" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -4838,7 +5036,7 @@
         <v>24</v>
       </c>
       <c r="D42" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -4852,7 +5050,7 @@
         <v>24</v>
       </c>
       <c r="D43" s="7">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -4944,9 +5142,181 @@
       <c r="C48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="7" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="8"/>
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
+      <c r="V57" s="8"/>
+      <c r="W57" s="8"/>
+      <c r="X57" s="8"/>
+      <c r="Y57" s="8"/>
+      <c r="Z57" s="8"/>
+      <c r="AA57" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -4972,27 +5342,27 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1">
         <v>50.0</v>
@@ -5006,10 +5376,10 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1">
         <v>100.0</v>
@@ -5018,15 +5388,15 @@
         <v>0.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1">
         <v>50.0</v>
@@ -5035,15 +5405,15 @@
         <v>0.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C5" s="1">
         <v>200000.0</v>
@@ -5052,15 +5422,15 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C6" s="1">
         <v>100.0</v>
@@ -5069,15 +5439,15 @@
         <v>2.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2">
         <v>150.0</v>
@@ -5086,15 +5456,15 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1">
         <v>150.0</v>
@@ -5103,15 +5473,15 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C9" s="2">
         <v>150.0</v>
@@ -5120,15 +5490,15 @@
         <v>2.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C10" s="1">
         <v>150.0</v>
@@ -5142,10 +5512,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C11" s="2">
         <v>275.0</v>
@@ -5154,15 +5524,15 @@
         <v>1.0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C12" s="2">
         <v>275.0</v>
@@ -5171,15 +5541,15 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C13" s="2">
         <v>275.0</v>
@@ -5193,10 +5563,10 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C14" s="2">
         <v>8000.0</v>
@@ -5210,10 +5580,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2">
         <v>12000.0</v>
@@ -5227,10 +5597,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C16" s="2">
         <v>10000.0</v>
@@ -5244,10 +5614,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C17" s="2">
         <v>240.0</v>
@@ -5261,10 +5631,10 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C18" s="1">
         <v>200.0</v>
@@ -5278,10 +5648,10 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C19" s="2">
         <v>1250.0</v>
@@ -5290,15 +5660,15 @@
         <v>1.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C20" s="2">
         <v>10.0</v>
@@ -5307,15 +5677,15 @@
         <v>0.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C21" s="2">
         <v>0.0</v>
@@ -5329,10 +5699,10 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C22" s="2">
         <v>0.0</v>
@@ -5341,15 +5711,15 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C23" s="2">
         <v>0.0</v>
@@ -5358,7 +5728,7 @@
         <v>0.0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1"/>
@@ -6367,7 +6737,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>99</v>
@@ -6376,13 +6746,13 @@
         <v>100</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -6405,7 +6775,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>101</v>
@@ -6414,18 +6784,18 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>101</v>
@@ -6434,18 +6804,18 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>101</v>
@@ -6454,18 +6824,18 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>101</v>
@@ -6474,56 +6844,56 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
+      <c r="D6" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
-        <v>142</v>
+      <c r="A7" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>110</v>
@@ -6532,18 +6902,18 @@
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="s">
-        <v>145</v>
+      <c r="A8" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>110</v>
@@ -6552,18 +6922,18 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
-        <v>146</v>
+      <c r="A9" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>110</v>
@@ -6572,18 +6942,18 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>110</v>
@@ -6592,18 +6962,18 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>110</v>
@@ -6612,10 +6982,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="F11" s="7">
         <v>0.0</v>
@@ -6641,7 +7011,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>115</v>
@@ -6650,18 +7020,18 @@
         <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>145</v>
+      <c r="A13" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>115</v>
@@ -6670,18 +7040,18 @@
         <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
-        <v>146</v>
+      <c r="A14" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>115</v>
@@ -6690,18 +7060,18 @@
         <v>85</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>115</v>
@@ -6710,18 +7080,18 @@
         <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>115</v>
@@ -6730,10 +7100,10 @@
         <v>85</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F16" s="7">
         <v>0.0</v>
@@ -6758,8 +7128,8 @@
       <c r="X16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
-        <v>145</v>
+      <c r="A17" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -6768,18 +7138,18 @@
         <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
-        <v>146</v>
+      <c r="A18" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -6788,18 +7158,18 @@
         <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>18</v>
@@ -6808,13 +7178,13 @@
         <v>85</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -6837,7 +7207,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>115</v>
@@ -6846,18 +7216,18 @@
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>115</v>
@@ -6866,18 +7236,18 @@
         <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>115</v>
@@ -6886,18 +7256,18 @@
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>115</v>
@@ -6906,18 +7276,18 @@
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>115</v>
@@ -6926,18 +7296,18 @@
         <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>115</v>
@@ -6946,18 +7316,18 @@
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>115</v>
@@ -6966,18 +7336,18 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>115</v>
@@ -6986,10 +7356,10 @@
         <v>24</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F27" s="7">
         <v>0.0</v>
@@ -7015,7 +7385,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>18</v>
@@ -7024,18 +7394,18 @@
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>18</v>
@@ -7044,18 +7414,18 @@
         <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>18</v>
@@ -7064,50 +7434,50 @@
         <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F32" s="2">
         <v>0.0</v>
@@ -7115,19 +7485,19 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F33" s="2">
         <v>0.0</v>
@@ -7135,19 +7505,19 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F34" s="2">
         <v>0.0</v>
@@ -7155,19 +7525,19 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F35" s="2">
         <v>0.0</v>
@@ -7196,13 +7566,13 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
@@ -8245,7 +8615,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>99</v>
@@ -8254,7 +8624,7 @@
         <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2">
@@ -8477,10 +8847,10 @@
         <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
@@ -8488,7 +8858,7 @@
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="C2" s="2">
         <v>150.0</v>
@@ -8499,7 +8869,7 @@
         <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C3" s="1">
         <v>0.05</v>

</xml_diff>

<commit_message>
lease size and cost of goods sold integrated
</commit_message>
<xml_diff>
--- a/Components_V2.xlsx
+++ b/Components_V2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="221">
   <si>
     <t>VariableName</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Lease Type</t>
   </si>
   <si>
-    <t>Standard</t>
+    <t>Standard Lease</t>
   </si>
   <si>
     <t>Longline Quantity</t>
@@ -430,7 +430,7 @@
     <t>`Longline Quantity` * 2</t>
   </si>
   <si>
-    <t>`Longline Quantity`*`Longline Depth`*2*`Mooring Length`</t>
+    <t>`Longline Quantity`*(`Longline Depth`-`Longline Suspended Depth`)*2*`Mooring Length`</t>
   </si>
   <si>
     <t>`Longline Quantity`*2</t>
@@ -616,10 +616,10 @@
     <t>ceiling(`Ear Hanging Droppers`/Labor.Subset$Task.Rate[i])</t>
   </si>
   <si>
-    <t>`Daily Work Hours` * Market.Product/Labor.Subset$Task.Rate[i]</t>
-  </si>
-  <si>
-    <t>ceiling(Market.Product/Labor.Subset$Task.Rate[i])</t>
+    <t>`Daily Work Hours` * Growth.Data$Market.Product/Labor.Subset$Task.Rate[i]</t>
+  </si>
+  <si>
+    <t>ceiling(Growth.Data$Market.Product/Labor.Subset$Task.Rate[i])</t>
   </si>
   <si>
     <t>12*Labor.Subset$Task.Rate[i]</t>
@@ -5659,8 +5659,9 @@
       <c r="D19" s="2">
         <v>1.0</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>150</v>
+      <c r="E19" s="2" t="str">
+        <f>Primary!B14</f>
+        <v>Fall</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -7447,8 +7448,9 @@
       <c r="A31" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>130</v>
+      <c r="B31" s="2" t="str">
+        <f>Primary!B15</f>
+        <v>Y3</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>131</v>

</xml_diff>